<commit_message>
Fix for Hebrew Calendar in DateTimePicker
</commit_message>
<xml_diff>
--- a/Resources/ZmanimFunctionList.xlsx
+++ b/Resources/ZmanimFunctionList.xlsx
@@ -2,10 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
-  <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2C29C46-FEE2-48E4-8503-6F4FC7791387}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub Project\MYZman\Resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23A90320-7E55-4BAF-A1FA-FBDA42A7929A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="35445" windowHeight="18255" xr2:uid="{67155520-7577-4C1A-98E8-EE8F939659DB}"/>
+    <workbookView xWindow="4125" yWindow="2430" windowWidth="26025" windowHeight="16680" xr2:uid="{67155520-7577-4C1A-98E8-EE8F939659DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Documentation list" sheetId="1" r:id="rId1"/>
@@ -2358,24 +2363,12 @@
     <t>beginning of bain hashmashos (twilight) according to the Yereim (Rabbi Eliezer of Metz) calculated as the sun's position 3.05° above the horizon during the equinox in Yerushalayim, its position 18 minutes or 3/4 of an 24 minute Mil before sunset. According to the Yereim, bain hashmashos starts 3/4 of a Mil before sunset and tzais or nightfall starts at sunset</t>
   </si>
   <si>
-    <t>Mincha gedola according to the Baal Hatanya based on true sunrise to sunset (see Sunrise Baal Hatanya)</t>
-  </si>
-  <si>
     <t>Baal Hatanya's shkiah amiti (see Sunrise Baal Hatanya)</t>
   </si>
   <si>
-    <t>מנחה גדולה לדעת בעל התניא המחושב לפי נץ ושקיעה אמתי (ראה עוד אצל נץ החמה לדעת בעל התניא)</t>
-  </si>
-  <si>
-    <t>פלג המנחה לדעת בעל התניא המחושב לפי נץ ושקיעה אמתי (ראה עוד אצל נץ החמה לדעת בעל התניא)</t>
-  </si>
-  <si>
     <t>In the winter when 1/2 of a shaah zmanis is less than 30 minutes Mincha Gedola 30 Minutes will be returned, otherwise Baal Hatanya's Mincha Gedola will be returned.</t>
   </si>
   <si>
-    <t>מנחה קטנה לדעת בעל התניא על פי נץ ושקיעה אמתי (ראה עוד אצל נץ החמה לבעל התניא)</t>
-  </si>
-  <si>
     <t>משיכיר מבוסס על מיקום השמש כשהיא 7.65 מעלות מתחת לאופק הגיאומטרי (90 דקות°).</t>
   </si>
   <si>
@@ -2388,27 +2381,6 @@
     <t>Misheyakir based on the position of the sun when it is 7.65° below geometric zenith (90 minutes°).</t>
   </si>
   <si>
-    <t>Mincha ketana according to the Baal Hatanya based on true sunrise to sunset (see Sunrise Baal Hatanya)</t>
-  </si>
-  <si>
-    <t>Plag Hamincha according to the Baal Hatanya based on true sunrise to sunset (see Sunrise Baal Hatanya)</t>
-  </si>
-  <si>
-    <t>Shaah Zmanis according to the Baal Hatanya based on true sunrise to sunset (see Sunrise Baal Hatanya)</t>
-  </si>
-  <si>
-    <t>Sof Zman Achilas Chametz according to the Baal Hatanya based on true sunrise to sunset (see Sunrise Baal Hatanya)</t>
-  </si>
-  <si>
-    <t>Sof Zman Biur Chametz according to the Baal Hatanya based on true sunrise to sunset (see Sunrise Baal Hatanya)</t>
-  </si>
-  <si>
-    <t>Sof Zman Shma according to the Baal Hatanya based on true sunrise to sunset (see Sunrise Baal Hatanya)</t>
-  </si>
-  <si>
-    <t>Sof Zman Tfila according to the Baal Hatanya based on true sunrise to sunset (see Sunrise Baal Hatanya)</t>
-  </si>
-  <si>
     <t>Tzais according to the Baal Hatanya based on the position of the sun 24 minutes after sunset in Jerusalem on the equinox (March 16, the day that a solar hour is 60 minutes), which is 6° below geometric zenith</t>
   </si>
   <si>
@@ -2916,9 +2888,6 @@
     <t>סו''ז תפילה לדעת בעל התניא</t>
   </si>
   <si>
-    <t>סו''ז תפילה לדעת בעל התניא המחושב לפי נץ ושקיעה אמתי (ראה עוד אצל נץ החמה לדעת בעל התניא)</t>
-  </si>
-  <si>
     <t>סו''ז שמע עטרת תורה</t>
   </si>
   <si>
@@ -2997,9 +2966,6 @@
     <t>סו''ז שמע לדעת בעל התניא</t>
   </si>
   <si>
-    <t>סו''ז שמע לדעת בעל התניא המחושב לפי נץ ושקיעה אמתי (ראה עוד אצל נץ החמה לדעת בעל התניא)</t>
-  </si>
-  <si>
     <t>סו''ז תפילה עטרת תורה</t>
   </si>
   <si>
@@ -3267,9 +3233,6 @@
     <t>סו''ז אכילת חמץ לדעת בעל התניא</t>
   </si>
   <si>
-    <t>סו''ז אכילת חמץ לדעת בעל התניא המחושב לפי נץ ושקיעה אמתי (ראה עוד אצל נץ החמה לדעת בעל התניא)</t>
-  </si>
-  <si>
     <t>סו''ז ביעור חמץ מג''א 16.1 מעלות</t>
   </si>
   <si>
@@ -3291,9 +3254,6 @@
     <t>סו''ז ביעור חמץ לדעת בעל התניא</t>
   </si>
   <si>
-    <t>סו''ז ביעור חמץ לדעת בעל התניא המחושב לפי נץ ושקיעה אמתי (ראה עוד אצל נץ החמה לדעת בעל התניא)</t>
-  </si>
-  <si>
     <t>Alos (dawn) calculated using 96 minutes zmaniyos or 1/7.5th of the day before sunrise or sea level sunrise.</t>
   </si>
   <si>
@@ -3307,6 +3267,51 @@
   </si>
   <si>
     <t>GetSofZmanAchilasChametzGRA</t>
+  </si>
+  <si>
+    <t>סו''ז שמע לדעת בעל התניא המחושב לפי נץ ושקיעה מותאם (ראה עוד אצל נץ החמה לדעת בעל התניא)</t>
+  </si>
+  <si>
+    <t>מנחה גדולה לדעת בעל התניא המחושב לפי נץ ושקיעה מותאם (ראה עוד אצל נץ החמה לדעת בעל התניא)</t>
+  </si>
+  <si>
+    <t>מנחה קטנה לדעת בעל התניא על פי נץ ושקיעה מותאם (ראה עוד אצל נץ החמה לבעל התניא)</t>
+  </si>
+  <si>
+    <t>פלג המנחה לדעת בעל התניא המחושב לפי נץ ושקיעה מותאם (ראה עוד אצל נץ החמה לדעת בעל התניא)</t>
+  </si>
+  <si>
+    <t>סו''ז אכילת חמץ לדעת בעל התניא המחושב לפי נץ ושקיעה מותאם (ראה עוד אצל נץ החמה לדעת בעל התניא)</t>
+  </si>
+  <si>
+    <t>סו''ז ביעור חמץ לדעת בעל התניא המחושב לפי נץ ושקיעה מותאם (ראה עוד אצל נץ החמה לדעת בעל התניא)</t>
+  </si>
+  <si>
+    <t>זמן התפילה האחרונה לדעת בעל התניא המחושב לפי נץ ושקיעה מותאם (ראה עוד אצל נץ החמה לדעת בעל התניא)</t>
+  </si>
+  <si>
+    <t>Sof Zman Shma according to the Baal Hatanya based on adjusted sunrise to sunset (see Sunrise Baal Hatanya)</t>
+  </si>
+  <si>
+    <t>Sof Zman Tfila according to the Baal Hatanya based on adjusted sunrise to sunset (see Sunrise Baal Hatanya)</t>
+  </si>
+  <si>
+    <t>Mincha gedola according to the Baal Hatanya based on adjusted sunrise to sunset (see Sunrise Baal Hatanya)</t>
+  </si>
+  <si>
+    <t>Mincha ketana according to the Baal Hatanya based on adjusted sunrise to sunset (see Sunrise Baal Hatanya)</t>
+  </si>
+  <si>
+    <t>Plag Hamincha according to the Baal Hatanya based on adjusted sunrise to sunset (see Sunrise Baal Hatanya)</t>
+  </si>
+  <si>
+    <t>Sof Zman Achilas Chametz according to the Baal Hatanya based on adjusted sunrise to sunset (see Sunrise Baal Hatanya)</t>
+  </si>
+  <si>
+    <t>Sof Zman Biur Chametz according to the Baal Hatanya based on adjusted sunrise to sunset (see Sunrise Baal Hatanya)</t>
+  </si>
+  <si>
+    <t>Shaah Zmanis according to the Baal Hatanya based on adjusted sunrise to sunset (see Sunrise Baal Hatanya)</t>
   </si>
 </sst>
 </file>
@@ -3943,10 +3948,10 @@
         <v>153</v>
       </c>
       <c r="E1" t="s">
-        <v>819</v>
+        <v>808</v>
       </c>
       <c r="F1" t="s">
-        <v>818</v>
+        <v>807</v>
       </c>
       <c r="G1" t="s">
         <v>120</v>
@@ -4006,13 +4011,13 @@
         <v>639</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>746</v>
+        <v>735</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>640</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>869</v>
+        <v>858</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>641</v>
@@ -4153,7 +4158,7 @@
         <v>250</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>1023</v>
+        <v>1008</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>106</v>
@@ -4199,7 +4204,7 @@
         <v>251</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>1025</v>
+        <v>1010</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>106</v>
@@ -4282,13 +4287,13 @@
         <v>643</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>747</v>
+        <v>736</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>669</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>815</v>
+        <v>804</v>
       </c>
       <c r="F16" s="7" t="s">
         <v>642</v>
@@ -4374,16 +4379,16 @@
         <v>676</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>758</v>
+        <v>747</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>677</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>718</v>
+        <v>714</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>719</v>
+        <v>715</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>106</v>
@@ -4397,16 +4402,16 @@
         <v>675</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>757</v>
+        <v>746</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>674</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>717</v>
+        <v>713</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>720</v>
+        <v>716</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>106</v>
@@ -4489,16 +4494,16 @@
         <v>644</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>765</v>
+        <v>754</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>670</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>814</v>
+        <v>803</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>813</v>
+        <v>802</v>
       </c>
       <c r="G25" s="4" t="s">
         <v>106</v>
@@ -4509,16 +4514,16 @@
         <v>25</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>825</v>
+        <v>814</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>463</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>870</v>
+        <v>859</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>871</v>
+        <v>860</v>
       </c>
       <c r="F26" s="4" t="s">
         <v>356</v>
@@ -4532,16 +4537,16 @@
         <v>26</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>826</v>
+        <v>815</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>462</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>872</v>
+        <v>861</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>873</v>
+        <v>862</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>355</v>
@@ -4555,16 +4560,16 @@
         <v>27</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>827</v>
+        <v>816</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>461</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>874</v>
+        <v>863</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>875</v>
+        <v>864</v>
       </c>
       <c r="F28" s="4" t="s">
         <v>354</v>
@@ -4584,13 +4589,13 @@
         <v>453</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>876</v>
+        <v>865</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>733</v>
+        <v>722</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>732</v>
+        <v>721</v>
       </c>
       <c r="G29" s="4" t="s">
         <v>106</v>
@@ -4607,10 +4612,10 @@
         <v>454</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>877</v>
+        <v>866</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>734</v>
+        <v>723</v>
       </c>
       <c r="F30" s="4" t="s">
         <v>197</v>
@@ -4624,16 +4629,16 @@
         <v>30</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>828</v>
+        <v>817</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>460</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>878</v>
+        <v>867</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>879</v>
+        <v>868</v>
       </c>
       <c r="F31" s="4" t="s">
         <v>353</v>
@@ -4647,16 +4652,16 @@
         <v>31</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>829</v>
+        <v>818</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>468</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>880</v>
+        <v>869</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>881</v>
+        <v>870</v>
       </c>
       <c r="F32" s="4" t="s">
         <v>361</v>
@@ -4670,16 +4675,16 @@
         <v>32</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>830</v>
+        <v>819</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>469</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>882</v>
+        <v>871</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>883</v>
+        <v>872</v>
       </c>
       <c r="F33" s="4" t="s">
         <v>362</v>
@@ -4693,16 +4698,16 @@
         <v>33</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>831</v>
+        <v>820</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>466</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>884</v>
+        <v>873</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>885</v>
+        <v>874</v>
       </c>
       <c r="F34" s="4" t="s">
         <v>359</v>
@@ -4716,16 +4721,16 @@
         <v>34</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>832</v>
+        <v>821</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>467</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>886</v>
+        <v>875</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>887</v>
+        <v>876</v>
       </c>
       <c r="F35" s="4" t="s">
         <v>360</v>
@@ -4739,16 +4744,16 @@
         <v>35</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>833</v>
+        <v>822</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>464</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>888</v>
+        <v>877</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>889</v>
+        <v>878</v>
       </c>
       <c r="F36" s="4" t="s">
         <v>357</v>
@@ -4762,16 +4767,16 @@
         <v>36</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>834</v>
+        <v>823</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>465</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>890</v>
+        <v>879</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>891</v>
+        <v>880</v>
       </c>
       <c r="F37" s="4" t="s">
         <v>358</v>
@@ -4785,19 +4790,19 @@
         <v>37</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>848</v>
+        <v>837</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>457</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>892</v>
+        <v>881</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>893</v>
+        <v>882</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>847</v>
+        <v>836</v>
       </c>
       <c r="G38" s="4" t="s">
         <v>106</v>
@@ -4814,13 +4819,13 @@
         <v>452</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>894</v>
+        <v>883</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>730</v>
+        <v>719</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>731</v>
+        <v>720</v>
       </c>
       <c r="G39" s="4" t="s">
         <v>106</v>
@@ -4831,19 +4836,19 @@
         <v>39</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>846</v>
+        <v>835</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>456</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>895</v>
+        <v>884</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>816</v>
+        <v>805</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>738</v>
+        <v>727</v>
       </c>
       <c r="G40" s="4" t="s">
         <v>106</v>
@@ -4857,16 +4862,16 @@
         <v>653</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>763</v>
+        <v>752</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>896</v>
+        <v>911</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>897</v>
+        <v>1013</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>726</v>
+        <v>1020</v>
       </c>
       <c r="G41" s="4" t="s">
         <v>106</v>
@@ -4883,13 +4888,13 @@
         <v>455</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>898</v>
+        <v>886</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>735</v>
+        <v>724</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>736</v>
+        <v>725</v>
       </c>
       <c r="G42" s="4" t="s">
         <v>106</v>
@@ -4900,16 +4905,16 @@
         <v>42</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>835</v>
+        <v>824</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>478</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>899</v>
+        <v>887</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>900</v>
+        <v>888</v>
       </c>
       <c r="F43" s="4" t="s">
         <v>366</v>
@@ -4923,16 +4928,16 @@
         <v>43</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>836</v>
+        <v>825</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>477</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>901</v>
+        <v>889</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>902</v>
+        <v>890</v>
       </c>
       <c r="F44" s="4" t="s">
         <v>365</v>
@@ -4946,16 +4951,16 @@
         <v>44</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>837</v>
+        <v>826</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>476</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>903</v>
+        <v>891</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>904</v>
+        <v>892</v>
       </c>
       <c r="F45" s="4" t="s">
         <v>364</v>
@@ -4969,16 +4974,16 @@
         <v>45</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>838</v>
+        <v>827</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>475</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>905</v>
+        <v>893</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>906</v>
+        <v>894</v>
       </c>
       <c r="F46" s="4" t="s">
         <v>363</v>
@@ -4992,16 +4997,16 @@
         <v>46</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>839</v>
+        <v>828</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>483</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>907</v>
+        <v>895</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>908</v>
+        <v>896</v>
       </c>
       <c r="F47" s="4" t="s">
         <v>371</v>
@@ -5015,16 +5020,16 @@
         <v>47</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>840</v>
+        <v>829</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>484</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>909</v>
+        <v>897</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>910</v>
+        <v>898</v>
       </c>
       <c r="F48" s="4" t="s">
         <v>372</v>
@@ -5038,16 +5043,16 @@
         <v>48</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>841</v>
+        <v>830</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>481</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>911</v>
+        <v>899</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>912</v>
+        <v>900</v>
       </c>
       <c r="F49" s="4" t="s">
         <v>369</v>
@@ -5061,16 +5066,16 @@
         <v>49</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>842</v>
+        <v>831</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>482</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>913</v>
+        <v>901</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>914</v>
+        <v>902</v>
       </c>
       <c r="F50" s="4" t="s">
         <v>370</v>
@@ -5084,16 +5089,16 @@
         <v>50</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>843</v>
+        <v>832</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>479</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>915</v>
+        <v>903</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>916</v>
+        <v>904</v>
       </c>
       <c r="F51" s="4" t="s">
         <v>367</v>
@@ -5107,16 +5112,16 @@
         <v>51</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>844</v>
+        <v>833</v>
       </c>
       <c r="C52" s="4" t="s">
         <v>480</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>917</v>
+        <v>905</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>918</v>
+        <v>906</v>
       </c>
       <c r="F52" s="4" t="s">
         <v>368</v>
@@ -5130,19 +5135,19 @@
         <v>52</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>850</v>
+        <v>839</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>472</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>919</v>
+        <v>907</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>920</v>
+        <v>908</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>851</v>
+        <v>840</v>
       </c>
       <c r="G53" s="4" t="s">
         <v>106</v>
@@ -5160,13 +5165,13 @@
         <v>470</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>921</v>
+        <v>909</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>817</v>
+        <v>806</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>740</v>
+        <v>729</v>
       </c>
       <c r="G54" s="4" t="s">
         <v>106</v>
@@ -5177,19 +5182,19 @@
         <v>54</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>821</v>
+        <v>810</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>471</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>922</v>
+        <v>910</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>775</v>
+        <v>764</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>739</v>
+        <v>728</v>
       </c>
       <c r="G55" s="4" t="s">
         <v>106</v>
@@ -5203,16 +5208,16 @@
         <v>654</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>764</v>
+        <v>753</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>923</v>
+        <v>885</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>924</v>
+        <v>1019</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>727</v>
+        <v>1021</v>
       </c>
       <c r="G56" s="4" t="s">
         <v>106</v>
@@ -5223,19 +5228,19 @@
         <v>56</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>403</v>
-      </c>
-      <c r="D57" s="4" t="s">
-        <v>175</v>
+        <v>473</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>912</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>268</v>
+        <v>730</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>271</v>
+        <v>731</v>
       </c>
       <c r="G57" s="4" t="s">
         <v>106</v>
@@ -5246,19 +5251,19 @@
         <v>57</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>127</v>
+        <v>86</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>473</v>
-      </c>
-      <c r="D58" s="5" t="s">
-        <v>925</v>
+        <v>84</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>173</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>741</v>
+        <v>630</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>742</v>
+        <v>190</v>
       </c>
       <c r="G58" s="4" t="s">
         <v>106</v>
@@ -5269,19 +5274,19 @@
         <v>58</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>86</v>
+        <v>811</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="D59" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="E59" s="5" t="s">
-        <v>630</v>
+        <v>398</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>703</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>726</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>190</v>
+        <v>704</v>
       </c>
       <c r="G59" s="4" t="s">
         <v>106</v>
@@ -5292,63 +5297,63 @@
         <v>59</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>822</v>
+        <v>262</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>703</v>
-      </c>
-      <c r="E60" s="4" t="s">
-        <v>737</v>
+        <v>913</v>
+      </c>
+      <c r="E60" s="5" t="s">
+        <v>914</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>704</v>
-      </c>
-      <c r="G60" s="4" t="s">
-        <v>106</v>
-      </c>
+        <v>267</v>
+      </c>
+      <c r="G60" s="4"/>
     </row>
     <row r="61" spans="1:8">
       <c r="A61" s="4">
         <v>60</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>262</v>
+        <v>148</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>399</v>
-      </c>
-      <c r="D61" s="5" t="s">
-        <v>926</v>
+        <v>401</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>174</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>927</v>
+        <v>266</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="G61" s="4"/>
+        <v>265</v>
+      </c>
+      <c r="G61" s="4" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="62" spans="1:8">
       <c r="A62" s="4">
         <v>61</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>148</v>
+        <v>176</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>401</v>
+        <v>404</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="E62" s="5" t="s">
-        <v>266</v>
+        <v>915</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="G62" s="4" t="s">
         <v>106</v>
@@ -5359,19 +5364,19 @@
         <v>62</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>176</v>
+        <v>263</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>177</v>
+        <v>916</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>928</v>
+        <v>917</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>264</v>
+        <v>209</v>
       </c>
       <c r="G63" s="4" t="s">
         <v>106</v>
@@ -5382,19 +5387,19 @@
         <v>63</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>263</v>
+        <v>100</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>929</v>
+        <v>834</v>
       </c>
       <c r="E64" s="5" t="s">
-        <v>930</v>
+        <v>918</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>209</v>
+        <v>191</v>
       </c>
       <c r="G64" s="4" t="s">
         <v>106</v>
@@ -5405,19 +5410,19 @@
         <v>64</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>100</v>
+        <v>647</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>400</v>
-      </c>
-      <c r="D65" s="4" t="s">
-        <v>845</v>
+        <v>743</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>668</v>
       </c>
       <c r="E65" s="5" t="s">
-        <v>931</v>
+        <v>1014</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>191</v>
+        <v>1022</v>
       </c>
       <c r="G65" s="4" t="s">
         <v>106</v>
@@ -5428,19 +5433,19 @@
         <v>65</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>647</v>
+        <v>656</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>754</v>
+        <v>744</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>668</v>
+        <v>673</v>
       </c>
       <c r="E66" s="5" t="s">
-        <v>713</v>
+        <v>771</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="G66" s="4" t="s">
         <v>106</v>
@@ -5451,19 +5456,19 @@
         <v>66</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>656</v>
+        <v>122</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>755</v>
-      </c>
-      <c r="D67" s="5" t="s">
-        <v>673</v>
+        <v>403</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>175</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>782</v>
+        <v>268</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>715</v>
+        <v>271</v>
       </c>
       <c r="G67" s="4" t="s">
         <v>106</v>
@@ -5474,19 +5479,19 @@
         <v>67</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>823</v>
+        <v>812</v>
       </c>
       <c r="C68" s="4" t="s">
         <v>405</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>932</v>
+        <v>919</v>
       </c>
       <c r="E68" s="5" t="s">
-        <v>933</v>
+        <v>920</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>824</v>
+        <v>813</v>
       </c>
       <c r="G68" s="4"/>
     </row>
@@ -5501,10 +5506,10 @@
         <v>407</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>934</v>
+        <v>921</v>
       </c>
       <c r="E69" s="5" t="s">
-        <v>935</v>
+        <v>922</v>
       </c>
       <c r="F69" s="4" t="s">
         <v>210</v>
@@ -5527,7 +5532,7 @@
         <v>178</v>
       </c>
       <c r="E70" s="5" t="s">
-        <v>936</v>
+        <v>923</v>
       </c>
       <c r="F70" s="4" t="s">
         <v>192</v>
@@ -5544,16 +5549,16 @@
         <v>648</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>756</v>
+        <v>745</v>
       </c>
       <c r="D71" s="5" t="s">
         <v>672</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>716</v>
+        <v>1015</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>721</v>
+        <v>1023</v>
       </c>
       <c r="G71" s="4" t="s">
         <v>106</v>
@@ -5691,7 +5696,7 @@
         <v>276</v>
       </c>
       <c r="F77" s="4" t="s">
-        <v>1026</v>
+        <v>1011</v>
       </c>
       <c r="G77" s="4" t="s">
         <v>106</v>
@@ -5757,7 +5762,7 @@
         <v>283</v>
       </c>
       <c r="E80" s="5" t="s">
-        <v>937</v>
+        <v>924</v>
       </c>
       <c r="F80" s="4" t="s">
         <v>211</v>
@@ -5803,7 +5808,7 @@
         <v>295</v>
       </c>
       <c r="E82" s="5" t="s">
-        <v>938</v>
+        <v>925</v>
       </c>
       <c r="F82" s="4" t="s">
         <v>216</v>
@@ -5826,7 +5831,7 @@
         <v>296</v>
       </c>
       <c r="E83" s="5" t="s">
-        <v>939</v>
+        <v>926</v>
       </c>
       <c r="F83" s="4" t="s">
         <v>227</v>
@@ -5849,7 +5854,7 @@
         <v>285</v>
       </c>
       <c r="E84" s="5" t="s">
-        <v>940</v>
+        <v>927</v>
       </c>
       <c r="F84" s="4" t="s">
         <v>215</v>
@@ -5872,7 +5877,7 @@
         <v>294</v>
       </c>
       <c r="E85" s="5" t="s">
-        <v>941</v>
+        <v>928</v>
       </c>
       <c r="F85" s="4" t="s">
         <v>226</v>
@@ -5895,7 +5900,7 @@
         <v>292</v>
       </c>
       <c r="E86" s="5" t="s">
-        <v>942</v>
+        <v>929</v>
       </c>
       <c r="F86" s="4" t="s">
         <v>214</v>
@@ -5918,7 +5923,7 @@
         <v>293</v>
       </c>
       <c r="E87" s="5" t="s">
-        <v>943</v>
+        <v>930</v>
       </c>
       <c r="F87" s="4" t="s">
         <v>225</v>
@@ -5941,7 +5946,7 @@
         <v>284</v>
       </c>
       <c r="E88" s="5" t="s">
-        <v>944</v>
+        <v>931</v>
       </c>
       <c r="F88" s="4" t="s">
         <v>213</v>
@@ -5955,19 +5960,19 @@
         <v>88</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>852</v>
+        <v>841</v>
       </c>
       <c r="C89" s="4" t="s">
         <v>414</v>
       </c>
       <c r="D89" s="5" t="s">
-        <v>945</v>
+        <v>932</v>
       </c>
       <c r="E89" s="5" t="s">
-        <v>946</v>
+        <v>933</v>
       </c>
       <c r="F89" s="4" t="s">
-        <v>853</v>
+        <v>842</v>
       </c>
       <c r="G89" s="4" t="s">
         <v>106</v>
@@ -5981,16 +5986,16 @@
         <v>649</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>759</v>
+        <v>748</v>
       </c>
       <c r="D90" s="5" t="s">
         <v>678</v>
       </c>
       <c r="E90" s="5" t="s">
-        <v>714</v>
+        <v>1016</v>
       </c>
       <c r="F90" s="4" t="s">
-        <v>722</v>
+        <v>1024</v>
       </c>
       <c r="G90" s="4" t="s">
         <v>106</v>
@@ -6027,13 +6032,13 @@
         <v>661</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>753</v>
+        <v>742</v>
       </c>
       <c r="D92" s="5" t="s">
         <v>667</v>
       </c>
       <c r="E92" s="4" t="s">
-        <v>781</v>
+        <v>770</v>
       </c>
       <c r="F92" s="1" t="s">
         <v>710</v>
@@ -6050,13 +6055,13 @@
         <v>660</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>752</v>
+        <v>741</v>
       </c>
       <c r="D93" s="5" t="s">
         <v>666</v>
       </c>
       <c r="E93" s="4" t="s">
-        <v>780</v>
+        <v>769</v>
       </c>
       <c r="F93" s="1" t="s">
         <v>709</v>
@@ -6073,13 +6078,13 @@
         <v>659</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>751</v>
+        <v>740</v>
       </c>
       <c r="D94" s="5" t="s">
         <v>665</v>
       </c>
       <c r="E94" s="4" t="s">
-        <v>779</v>
+        <v>768</v>
       </c>
       <c r="F94" s="1" t="s">
         <v>708</v>
@@ -6096,13 +6101,13 @@
         <v>655</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>750</v>
+        <v>739</v>
       </c>
       <c r="D95" s="5" t="s">
         <v>663</v>
       </c>
       <c r="E95" s="4" t="s">
-        <v>778</v>
+        <v>767</v>
       </c>
       <c r="F95" s="1" t="s">
         <v>707</v>
@@ -6119,13 +6124,13 @@
         <v>658</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>749</v>
+        <v>738</v>
       </c>
       <c r="D96" s="5" t="s">
         <v>664</v>
       </c>
       <c r="E96" s="4" t="s">
-        <v>777</v>
+        <v>766</v>
       </c>
       <c r="F96" s="1" t="s">
         <v>706</v>
@@ -6142,13 +6147,13 @@
         <v>657</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>748</v>
+        <v>737</v>
       </c>
       <c r="D97" s="5" t="s">
         <v>662</v>
       </c>
       <c r="E97" s="4" t="s">
-        <v>776</v>
+        <v>765</v>
       </c>
       <c r="F97" s="1" t="s">
         <v>705</v>
@@ -6162,7 +6167,7 @@
         <v>97</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>820</v>
+        <v>809</v>
       </c>
       <c r="C98" s="4" t="s">
         <v>487</v>
@@ -6211,16 +6216,16 @@
         <v>645</v>
       </c>
       <c r="C100" s="6" t="s">
-        <v>766</v>
+        <v>755</v>
       </c>
       <c r="D100" s="5" t="s">
         <v>671</v>
       </c>
       <c r="E100" s="4" t="s">
-        <v>812</v>
+        <v>801</v>
       </c>
       <c r="F100" s="4" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="G100" s="4" t="s">
         <v>106</v>
@@ -6237,10 +6242,10 @@
         <v>504</v>
       </c>
       <c r="D101" s="5" t="s">
-        <v>947</v>
+        <v>934</v>
       </c>
       <c r="E101" s="5" t="s">
-        <v>948</v>
+        <v>935</v>
       </c>
       <c r="F101" s="1" t="s">
         <v>695</v>
@@ -6260,10 +6265,10 @@
         <v>505</v>
       </c>
       <c r="D102" s="5" t="s">
-        <v>949</v>
+        <v>936</v>
       </c>
       <c r="E102" s="5" t="s">
-        <v>950</v>
+        <v>937</v>
       </c>
       <c r="F102" s="1" t="s">
         <v>696</v>
@@ -6277,16 +6282,16 @@
         <v>102</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>859</v>
+        <v>848</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>768</v>
+        <v>757</v>
       </c>
       <c r="D103" s="5" t="s">
-        <v>951</v>
+        <v>938</v>
       </c>
       <c r="E103" s="5" t="s">
-        <v>952</v>
+        <v>939</v>
       </c>
       <c r="F103" s="1" t="s">
         <v>689</v>
@@ -6300,16 +6305,16 @@
         <v>103</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>860</v>
+        <v>849</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>769</v>
+        <v>758</v>
       </c>
       <c r="D104" s="5" t="s">
-        <v>953</v>
+        <v>940</v>
       </c>
       <c r="E104" s="5" t="s">
-        <v>954</v>
+        <v>941</v>
       </c>
       <c r="F104" s="1" t="s">
         <v>690</v>
@@ -6329,10 +6334,10 @@
         <v>506</v>
       </c>
       <c r="D105" s="5" t="s">
-        <v>955</v>
+        <v>942</v>
       </c>
       <c r="E105" s="5" t="s">
-        <v>956</v>
+        <v>943</v>
       </c>
       <c r="F105" s="1" t="s">
         <v>697</v>
@@ -6352,10 +6357,10 @@
         <v>507</v>
       </c>
       <c r="D106" s="5" t="s">
-        <v>957</v>
+        <v>944</v>
       </c>
       <c r="E106" s="5" t="s">
-        <v>958</v>
+        <v>945</v>
       </c>
       <c r="F106" s="1" t="s">
         <v>698</v>
@@ -6375,10 +6380,10 @@
         <v>508</v>
       </c>
       <c r="D107" s="5" t="s">
-        <v>959</v>
+        <v>946</v>
       </c>
       <c r="E107" s="5" t="s">
-        <v>960</v>
+        <v>947</v>
       </c>
       <c r="F107" s="1" t="s">
         <v>699</v>
@@ -6398,10 +6403,10 @@
         <v>509</v>
       </c>
       <c r="D108" s="5" t="s">
-        <v>961</v>
+        <v>948</v>
       </c>
       <c r="E108" s="5" t="s">
-        <v>962</v>
+        <v>949</v>
       </c>
       <c r="F108" s="1" t="s">
         <v>700</v>
@@ -6421,10 +6426,10 @@
         <v>510</v>
       </c>
       <c r="D109" s="5" t="s">
-        <v>963</v>
+        <v>950</v>
       </c>
       <c r="E109" s="5" t="s">
-        <v>964</v>
+        <v>951</v>
       </c>
       <c r="F109" s="1" t="s">
         <v>701</v>
@@ -6438,16 +6443,16 @@
         <v>109</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>861</v>
+        <v>850</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>770</v>
+        <v>759</v>
       </c>
       <c r="D110" s="5" t="s">
-        <v>965</v>
+        <v>952</v>
       </c>
       <c r="E110" s="5" t="s">
-        <v>966</v>
+        <v>953</v>
       </c>
       <c r="F110" s="1" t="s">
         <v>691</v>
@@ -6467,10 +6472,10 @@
         <v>511</v>
       </c>
       <c r="D111" s="5" t="s">
-        <v>967</v>
+        <v>954</v>
       </c>
       <c r="E111" s="5" t="s">
-        <v>968</v>
+        <v>955</v>
       </c>
       <c r="F111" s="4" t="s">
         <v>702</v>
@@ -6484,16 +6489,16 @@
         <v>111</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>862</v>
+        <v>851</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>771</v>
+        <v>760</v>
       </c>
       <c r="D112" s="5" t="s">
-        <v>969</v>
+        <v>956</v>
       </c>
       <c r="E112" s="5" t="s">
-        <v>970</v>
+        <v>957</v>
       </c>
       <c r="F112" s="1" t="s">
         <v>692</v>
@@ -6513,10 +6518,10 @@
         <v>512</v>
       </c>
       <c r="D113" s="5" t="s">
-        <v>971</v>
+        <v>958</v>
       </c>
       <c r="E113" s="5" t="s">
-        <v>972</v>
+        <v>959</v>
       </c>
       <c r="F113" s="4" t="s">
         <v>203</v>
@@ -6530,16 +6535,16 @@
         <v>113</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>863</v>
+        <v>852</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>772</v>
+        <v>761</v>
       </c>
       <c r="D114" s="5" t="s">
-        <v>973</v>
+        <v>960</v>
       </c>
       <c r="E114" s="5" t="s">
-        <v>974</v>
+        <v>961</v>
       </c>
       <c r="F114" s="1" t="s">
         <v>693</v>
@@ -6553,16 +6558,16 @@
         <v>114</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>864</v>
+        <v>853</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>773</v>
+        <v>762</v>
       </c>
       <c r="D115" s="5" t="s">
-        <v>975</v>
+        <v>962</v>
       </c>
       <c r="E115" s="5" t="s">
-        <v>976</v>
+        <v>963</v>
       </c>
       <c r="F115" s="1" t="s">
         <v>694</v>
@@ -6582,10 +6587,10 @@
         <v>492</v>
       </c>
       <c r="D116" s="5" t="s">
-        <v>977</v>
+        <v>964</v>
       </c>
       <c r="E116" s="5" t="s">
-        <v>978</v>
+        <v>965</v>
       </c>
       <c r="F116" s="4" t="s">
         <v>199</v>
@@ -6605,10 +6610,10 @@
         <v>493</v>
       </c>
       <c r="D117" s="5" t="s">
-        <v>979</v>
+        <v>966</v>
       </c>
       <c r="E117" s="5" t="s">
-        <v>980</v>
+        <v>967</v>
       </c>
       <c r="F117" s="4" t="s">
         <v>200</v>
@@ -6628,10 +6633,10 @@
         <v>494</v>
       </c>
       <c r="D118" s="5" t="s">
-        <v>981</v>
+        <v>968</v>
       </c>
       <c r="E118" s="5" t="s">
-        <v>982</v>
+        <v>969</v>
       </c>
       <c r="F118" s="4" t="s">
         <v>201</v>
@@ -6651,10 +6656,10 @@
         <v>495</v>
       </c>
       <c r="D119" s="5" t="s">
-        <v>983</v>
+        <v>970</v>
       </c>
       <c r="E119" s="5" t="s">
-        <v>984</v>
+        <v>971</v>
       </c>
       <c r="F119" s="4" t="s">
         <v>202</v>
@@ -6674,10 +6679,10 @@
         <v>496</v>
       </c>
       <c r="D120" s="5" t="s">
-        <v>985</v>
+        <v>972</v>
       </c>
       <c r="E120" s="5" t="s">
-        <v>986</v>
+        <v>973</v>
       </c>
       <c r="F120" s="4" t="s">
         <v>219</v>
@@ -6720,10 +6725,10 @@
         <v>498</v>
       </c>
       <c r="D122" s="5" t="s">
-        <v>987</v>
+        <v>974</v>
       </c>
       <c r="E122" s="5" t="s">
-        <v>988</v>
+        <v>975</v>
       </c>
       <c r="F122" s="4" t="s">
         <v>220</v>
@@ -6743,10 +6748,10 @@
         <v>499</v>
       </c>
       <c r="D123" s="5" t="s">
-        <v>989</v>
+        <v>976</v>
       </c>
       <c r="E123" s="5" t="s">
-        <v>990</v>
+        <v>977</v>
       </c>
       <c r="F123" s="4" t="s">
         <v>221</v>
@@ -6766,10 +6771,10 @@
         <v>500</v>
       </c>
       <c r="D124" s="5" t="s">
-        <v>991</v>
+        <v>978</v>
       </c>
       <c r="E124" s="5" t="s">
-        <v>992</v>
+        <v>979</v>
       </c>
       <c r="F124" s="4" t="s">
         <v>222</v>
@@ -6789,10 +6794,10 @@
         <v>501</v>
       </c>
       <c r="D125" s="5" t="s">
-        <v>993</v>
+        <v>980</v>
       </c>
       <c r="E125" s="5" t="s">
-        <v>994</v>
+        <v>981</v>
       </c>
       <c r="F125" s="4" t="s">
         <v>223</v>
@@ -6812,10 +6817,10 @@
         <v>502</v>
       </c>
       <c r="D126" s="5" t="s">
-        <v>995</v>
+        <v>982</v>
       </c>
       <c r="E126" s="5" t="s">
-        <v>996</v>
+        <v>983</v>
       </c>
       <c r="F126" s="4" t="s">
         <v>224</v>
@@ -6835,10 +6840,10 @@
         <v>490</v>
       </c>
       <c r="D127" s="5" t="s">
-        <v>997</v>
+        <v>984</v>
       </c>
       <c r="E127" s="5" t="s">
-        <v>998</v>
+        <v>985</v>
       </c>
       <c r="F127" s="4" t="s">
         <v>217</v>
@@ -6858,10 +6863,10 @@
         <v>491</v>
       </c>
       <c r="D128" s="5" t="s">
-        <v>999</v>
+        <v>986</v>
       </c>
       <c r="E128" s="5" t="s">
-        <v>1000</v>
+        <v>987</v>
       </c>
       <c r="F128" s="4" t="s">
         <v>218</v>
@@ -6878,16 +6883,16 @@
         <v>646</v>
       </c>
       <c r="C129" s="4" t="s">
-        <v>767</v>
+        <v>756</v>
       </c>
       <c r="D129" s="5" t="s">
-        <v>1001</v>
+        <v>988</v>
       </c>
       <c r="E129" s="5" t="s">
-        <v>1002</v>
+        <v>989</v>
       </c>
       <c r="F129" s="4" t="s">
-        <v>728</v>
+        <v>717</v>
       </c>
       <c r="G129" s="4" t="s">
         <v>106</v>
@@ -6904,13 +6909,13 @@
         <v>503</v>
       </c>
       <c r="D130" s="5" t="s">
-        <v>1003</v>
+        <v>990</v>
       </c>
       <c r="E130" s="5" t="s">
-        <v>1024</v>
+        <v>1009</v>
       </c>
       <c r="F130" s="4" t="s">
-        <v>745</v>
+        <v>734</v>
       </c>
       <c r="G130" s="4" t="s">
         <v>106</v>
@@ -6996,7 +7001,7 @@
         <v>228</v>
       </c>
       <c r="D134" s="4" t="s">
-        <v>774</v>
+        <v>763</v>
       </c>
       <c r="E134" s="5" t="s">
         <v>635</v>
@@ -7065,10 +7070,10 @@
         <v>485</v>
       </c>
       <c r="D137" s="5" t="s">
-        <v>743</v>
+        <v>732</v>
       </c>
       <c r="E137" s="5" t="s">
-        <v>744</v>
+        <v>733</v>
       </c>
       <c r="F137" s="4" t="s">
         <v>198</v>
@@ -7082,19 +7087,19 @@
         <v>137</v>
       </c>
       <c r="B138" s="4" t="s">
+        <v>775</v>
+      </c>
+      <c r="C138" s="4" t="s">
+        <v>781</v>
+      </c>
+      <c r="D138" s="5" t="s">
         <v>786</v>
       </c>
-      <c r="C138" s="4" t="s">
-        <v>792</v>
-      </c>
-      <c r="D138" s="5" t="s">
-        <v>797</v>
-      </c>
       <c r="E138" s="4" t="s">
-        <v>798</v>
+        <v>787</v>
       </c>
       <c r="F138" s="7" t="s">
-        <v>799</v>
+        <v>788</v>
       </c>
       <c r="G138" s="4" t="s">
         <v>108</v>
@@ -7105,19 +7110,19 @@
         <v>138</v>
       </c>
       <c r="B139" s="4" t="s">
-        <v>783</v>
+        <v>772</v>
       </c>
       <c r="C139" s="4" t="s">
         <v>394</v>
       </c>
       <c r="D139" s="5" t="s">
-        <v>784</v>
+        <v>773</v>
       </c>
       <c r="E139" s="4" t="s">
-        <v>796</v>
+        <v>785</v>
       </c>
       <c r="F139" s="7" t="s">
-        <v>785</v>
+        <v>774</v>
       </c>
       <c r="G139" s="4" t="s">
         <v>106</v>
@@ -7128,19 +7133,19 @@
         <v>139</v>
       </c>
       <c r="B140" s="4" t="s">
-        <v>787</v>
+        <v>776</v>
       </c>
       <c r="C140" s="4" t="s">
-        <v>793</v>
+        <v>782</v>
       </c>
       <c r="D140" s="5" t="s">
-        <v>800</v>
+        <v>789</v>
       </c>
       <c r="E140" s="4" t="s">
-        <v>801</v>
+        <v>790</v>
       </c>
       <c r="F140" s="7" t="s">
-        <v>802</v>
+        <v>791</v>
       </c>
       <c r="G140" s="4" t="s">
         <v>108</v>
@@ -7151,19 +7156,19 @@
         <v>140</v>
       </c>
       <c r="B141" s="4" t="s">
-        <v>788</v>
+        <v>777</v>
       </c>
       <c r="C141" s="4" t="s">
+        <v>783</v>
+      </c>
+      <c r="D141" s="5" t="s">
+        <v>792</v>
+      </c>
+      <c r="E141" s="4" t="s">
+        <v>793</v>
+      </c>
+      <c r="F141" s="7" t="s">
         <v>794</v>
-      </c>
-      <c r="D141" s="5" t="s">
-        <v>803</v>
-      </c>
-      <c r="E141" s="4" t="s">
-        <v>804</v>
-      </c>
-      <c r="F141" s="7" t="s">
-        <v>805</v>
       </c>
       <c r="G141" s="4" t="s">
         <v>108</v>
@@ -7174,19 +7179,19 @@
         <v>141</v>
       </c>
       <c r="B142" s="4" t="s">
-        <v>789</v>
+        <v>778</v>
       </c>
       <c r="C142" s="4" t="s">
+        <v>784</v>
+      </c>
+      <c r="D142" s="5" t="s">
         <v>795</v>
       </c>
-      <c r="D142" s="5" t="s">
-        <v>806</v>
-      </c>
       <c r="E142" s="4" t="s">
-        <v>807</v>
+        <v>796</v>
       </c>
       <c r="F142" s="7" t="s">
-        <v>808</v>
+        <v>797</v>
       </c>
       <c r="G142" s="4" t="s">
         <v>108</v>
@@ -7197,19 +7202,19 @@
         <v>142</v>
       </c>
       <c r="B143" s="4" t="s">
-        <v>790</v>
+        <v>779</v>
       </c>
       <c r="C143" s="4" t="s">
-        <v>791</v>
+        <v>780</v>
       </c>
       <c r="D143" s="5" t="s">
-        <v>809</v>
+        <v>798</v>
       </c>
       <c r="E143" s="4" t="s">
-        <v>810</v>
+        <v>799</v>
       </c>
       <c r="F143" s="7" t="s">
-        <v>811</v>
+        <v>800</v>
       </c>
       <c r="G143" s="4" t="s">
         <v>108</v>
@@ -7220,16 +7225,16 @@
         <v>143</v>
       </c>
       <c r="B144" s="4" t="s">
-        <v>865</v>
+        <v>854</v>
       </c>
       <c r="C144" s="4" t="s">
         <v>447</v>
       </c>
       <c r="D144" s="5" t="s">
-        <v>1007</v>
+        <v>994</v>
       </c>
       <c r="E144" s="5" t="s">
-        <v>1008</v>
+        <v>995</v>
       </c>
       <c r="F144" s="4" t="s">
         <v>349</v>
@@ -7243,16 +7248,16 @@
         <v>144</v>
       </c>
       <c r="B145" s="4" t="s">
-        <v>866</v>
+        <v>855</v>
       </c>
       <c r="C145" s="4" t="s">
         <v>448</v>
       </c>
       <c r="D145" s="5" t="s">
-        <v>1009</v>
+        <v>996</v>
       </c>
       <c r="E145" s="5" t="s">
-        <v>1010</v>
+        <v>997</v>
       </c>
       <c r="F145" s="4" t="s">
         <v>350</v>
@@ -7266,16 +7271,16 @@
         <v>145</v>
       </c>
       <c r="B146" s="4" t="s">
-        <v>857</v>
+        <v>846</v>
       </c>
       <c r="C146" s="4" t="s">
-        <v>1027</v>
+        <v>1012</v>
       </c>
       <c r="D146" s="5" t="s">
-        <v>1011</v>
+        <v>998</v>
       </c>
       <c r="E146" s="5" t="s">
-        <v>1012</v>
+        <v>999</v>
       </c>
       <c r="F146" s="4" t="s">
         <v>195</v>
@@ -7292,16 +7297,16 @@
         <v>651</v>
       </c>
       <c r="C147" s="4" t="s">
-        <v>761</v>
+        <v>750</v>
       </c>
       <c r="D147" s="5" t="s">
-        <v>1013</v>
+        <v>1000</v>
       </c>
       <c r="E147" s="5" t="s">
-        <v>1014</v>
+        <v>1017</v>
       </c>
       <c r="F147" s="4" t="s">
-        <v>724</v>
+        <v>1025</v>
       </c>
       <c r="G147" s="4" t="s">
         <v>106</v>
@@ -7312,16 +7317,16 @@
         <v>147</v>
       </c>
       <c r="B148" s="4" t="s">
-        <v>867</v>
+        <v>856</v>
       </c>
       <c r="C148" s="4" t="s">
         <v>450</v>
       </c>
       <c r="D148" s="5" t="s">
-        <v>1015</v>
+        <v>1001</v>
       </c>
       <c r="E148" s="5" t="s">
-        <v>1016</v>
+        <v>1002</v>
       </c>
       <c r="F148" s="4" t="s">
         <v>351</v>
@@ -7335,16 +7340,16 @@
         <v>148</v>
       </c>
       <c r="B149" s="4" t="s">
-        <v>868</v>
+        <v>857</v>
       </c>
       <c r="C149" s="4" t="s">
         <v>451</v>
       </c>
       <c r="D149" s="5" t="s">
-        <v>1017</v>
+        <v>1003</v>
       </c>
       <c r="E149" s="5" t="s">
-        <v>1018</v>
+        <v>1004</v>
       </c>
       <c r="F149" s="4" t="s">
         <v>352</v>
@@ -7358,16 +7363,16 @@
         <v>149</v>
       </c>
       <c r="B150" s="4" t="s">
-        <v>858</v>
+        <v>847</v>
       </c>
       <c r="C150" s="4" t="s">
         <v>449</v>
       </c>
       <c r="D150" s="5" t="s">
-        <v>1019</v>
+        <v>1005</v>
       </c>
       <c r="E150" s="5" t="s">
-        <v>1020</v>
+        <v>1006</v>
       </c>
       <c r="F150" s="4" t="s">
         <v>196</v>
@@ -7384,16 +7389,16 @@
         <v>652</v>
       </c>
       <c r="C151" s="4" t="s">
-        <v>762</v>
+        <v>751</v>
       </c>
       <c r="D151" s="5" t="s">
-        <v>1021</v>
+        <v>1007</v>
       </c>
       <c r="E151" s="5" t="s">
-        <v>1022</v>
+        <v>1018</v>
       </c>
       <c r="F151" s="4" t="s">
-        <v>725</v>
+        <v>1026</v>
       </c>
       <c r="G151" s="4" t="s">
         <v>106</v>
@@ -7528,7 +7533,7 @@
         <v>303</v>
       </c>
       <c r="E157" s="5" t="s">
-        <v>1004</v>
+        <v>991</v>
       </c>
       <c r="F157" s="4" t="s">
         <v>343</v>
@@ -7692,7 +7697,7 @@
         <v>335</v>
       </c>
       <c r="F164" s="4" t="s">
-        <v>729</v>
+        <v>718</v>
       </c>
       <c r="G164" s="4" t="s">
         <v>106</v>
@@ -7703,19 +7708,19 @@
         <v>164</v>
       </c>
       <c r="B165" s="4" t="s">
-        <v>854</v>
+        <v>843</v>
       </c>
       <c r="C165" s="4" t="s">
         <v>445</v>
       </c>
       <c r="D165" s="5" t="s">
-        <v>1005</v>
+        <v>992</v>
       </c>
       <c r="E165" s="5" t="s">
-        <v>1006</v>
+        <v>993</v>
       </c>
       <c r="F165" s="4" t="s">
-        <v>856</v>
+        <v>845</v>
       </c>
       <c r="G165" s="4" t="s">
         <v>106</v>
@@ -7729,16 +7734,16 @@
         <v>650</v>
       </c>
       <c r="C166" s="4" t="s">
-        <v>760</v>
+        <v>749</v>
       </c>
       <c r="D166" s="5" t="s">
         <v>679</v>
       </c>
       <c r="E166" s="5" t="s">
-        <v>855</v>
+        <v>844</v>
       </c>
       <c r="F166" s="4" t="s">
-        <v>723</v>
+        <v>1027</v>
       </c>
       <c r="G166" s="4" t="s">
         <v>106</v>
@@ -7832,7 +7837,7 @@
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>849</v>
+        <v>838</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -8026,7 +8031,7 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>746</v>
+        <v>735</v>
       </c>
       <c r="B26" t="b">
         <f>COUNTIF('Documentation list'!C:C,Table2[[#This Row],[list from dll]])&gt;0</f>
@@ -8116,7 +8121,7 @@
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>747</v>
+        <v>736</v>
       </c>
       <c r="B36" t="b">
         <f>COUNTIF('Documentation list'!C:C,Table2[[#This Row],[list from dll]])&gt;0</f>
@@ -8161,7 +8166,7 @@
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>748</v>
+        <v>737</v>
       </c>
       <c r="B41" t="b">
         <f>COUNTIF('Documentation list'!C:C,Table2[[#This Row],[list from dll]])&gt;0</f>
@@ -8170,7 +8175,7 @@
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>749</v>
+        <v>738</v>
       </c>
       <c r="B42" t="b">
         <f>COUNTIF('Documentation list'!C:C,Table2[[#This Row],[list from dll]])&gt;0</f>
@@ -8179,7 +8184,7 @@
     </row>
     <row r="43" spans="1:2">
       <c r="A43" t="s">
-        <v>750</v>
+        <v>739</v>
       </c>
       <c r="B43" t="b">
         <f>COUNTIF('Documentation list'!C:C,Table2[[#This Row],[list from dll]])&gt;0</f>
@@ -8188,7 +8193,7 @@
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>751</v>
+        <v>740</v>
       </c>
       <c r="B44" t="b">
         <f>COUNTIF('Documentation list'!C:C,Table2[[#This Row],[list from dll]])&gt;0</f>
@@ -8197,7 +8202,7 @@
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>752</v>
+        <v>741</v>
       </c>
       <c r="B45" s="2" t="b">
         <f>COUNTIF('Documentation list'!C:C,Table2[[#This Row],[list from dll]])&gt;0</f>
@@ -8206,7 +8211,7 @@
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>753</v>
+        <v>742</v>
       </c>
       <c r="B46" t="b">
         <f>COUNTIF('Documentation list'!C:C,Table2[[#This Row],[list from dll]])&gt;0</f>
@@ -8287,7 +8292,7 @@
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>754</v>
+        <v>743</v>
       </c>
       <c r="B55" t="b">
         <f>COUNTIF('Documentation list'!C:C,Table2[[#This Row],[list from dll]])&gt;0</f>
@@ -8296,7 +8301,7 @@
     </row>
     <row r="56" spans="1:2">
       <c r="A56" t="s">
-        <v>755</v>
+        <v>744</v>
       </c>
       <c r="B56" t="b">
         <f>COUNTIF('Documentation list'!C:C,Table2[[#This Row],[list from dll]])&gt;0</f>
@@ -8341,7 +8346,7 @@
     </row>
     <row r="61" spans="1:2">
       <c r="A61" t="s">
-        <v>756</v>
+        <v>745</v>
       </c>
       <c r="B61" t="b">
         <f>COUNTIF('Documentation list'!C:C,Table2[[#This Row],[list from dll]])&gt;0</f>
@@ -8377,7 +8382,7 @@
     </row>
     <row r="65" spans="1:2">
       <c r="A65" t="s">
-        <v>757</v>
+        <v>746</v>
       </c>
       <c r="B65" t="b">
         <f>COUNTIF('Documentation list'!C:C,Table2[[#This Row],[list from dll]])&gt;0</f>
@@ -8386,7 +8391,7 @@
     </row>
     <row r="66" spans="1:2">
       <c r="A66" t="s">
-        <v>758</v>
+        <v>747</v>
       </c>
       <c r="B66" t="b">
         <f>COUNTIF('Documentation list'!C:C,Table2[[#This Row],[list from dll]])&gt;0</f>
@@ -8539,7 +8544,7 @@
     </row>
     <row r="83" spans="1:2">
       <c r="A83" t="s">
-        <v>759</v>
+        <v>748</v>
       </c>
       <c r="B83" t="b">
         <f>COUNTIF('Documentation list'!C:C,Table2[[#This Row],[list from dll]])&gt;0</f>
@@ -8692,7 +8697,7 @@
     </row>
     <row r="100" spans="1:2">
       <c r="A100" t="s">
-        <v>760</v>
+        <v>749</v>
       </c>
       <c r="B100" t="b">
         <f>COUNTIF('Documentation list'!C:C,Table2[[#This Row],[list from dll]])&gt;0</f>
@@ -8701,7 +8706,7 @@
     </row>
     <row r="101" spans="1:2">
       <c r="A101" t="s">
-        <v>761</v>
+        <v>750</v>
       </c>
       <c r="B101" t="b">
         <f>COUNTIF('Documentation list'!C:C,Table2[[#This Row],[list from dll]])&gt;0</f>
@@ -8737,7 +8742,7 @@
     </row>
     <row r="105" spans="1:2">
       <c r="A105" t="s">
-        <v>762</v>
+        <v>751</v>
       </c>
       <c r="B105" t="b">
         <f>COUNTIF('Documentation list'!C:C,Table2[[#This Row],[list from dll]])&gt;0</f>
@@ -8809,7 +8814,7 @@
     </row>
     <row r="113" spans="1:2">
       <c r="A113" t="s">
-        <v>763</v>
+        <v>752</v>
       </c>
       <c r="B113" t="b">
         <f>COUNTIF('Documentation list'!C:C,Table2[[#This Row],[list from dll]])&gt;0</f>
@@ -8926,7 +8931,7 @@
     </row>
     <row r="126" spans="1:2">
       <c r="A126" t="s">
-        <v>764</v>
+        <v>753</v>
       </c>
       <c r="B126" t="b">
         <f>COUNTIF('Documentation list'!C:C,Table2[[#This Row],[list from dll]])&gt;0</f>
@@ -9061,7 +9066,7 @@
     </row>
     <row r="141" spans="1:2">
       <c r="A141" t="s">
-        <v>765</v>
+        <v>754</v>
       </c>
       <c r="B141" t="b">
         <f>COUNTIF('Documentation list'!C:C,Table2[[#This Row],[list from dll]])&gt;0</f>
@@ -9079,7 +9084,7 @@
     </row>
     <row r="143" spans="1:2">
       <c r="A143" t="s">
-        <v>766</v>
+        <v>755</v>
       </c>
       <c r="B143" t="b">
         <f>COUNTIF('Documentation list'!C:C,Table2[[#This Row],[list from dll]])&gt;0</f>
@@ -9214,7 +9219,7 @@
     </row>
     <row r="158" spans="1:2">
       <c r="A158" t="s">
-        <v>767</v>
+        <v>756</v>
       </c>
       <c r="B158" s="3" t="b">
         <f>COUNTIF('Documentation list'!C:C,Table2[[#This Row],[list from dll]])&gt;0</f>
@@ -9241,7 +9246,7 @@
     </row>
     <row r="161" spans="1:2">
       <c r="A161" t="s">
-        <v>768</v>
+        <v>757</v>
       </c>
       <c r="B161" s="3" t="b">
         <f>COUNTIF('Documentation list'!C:C,Table2[[#This Row],[list from dll]])&gt;0</f>
@@ -9250,7 +9255,7 @@
     </row>
     <row r="162" spans="1:2">
       <c r="A162" t="s">
-        <v>769</v>
+        <v>758</v>
       </c>
       <c r="B162" s="3" t="b">
         <f>COUNTIF('Documentation list'!C:C,Table2[[#This Row],[list from dll]])&gt;0</f>
@@ -9304,7 +9309,7 @@
     </row>
     <row r="168" spans="1:2">
       <c r="A168" t="s">
-        <v>770</v>
+        <v>759</v>
       </c>
       <c r="B168" s="3" t="b">
         <f>COUNTIF('Documentation list'!C:C,Table2[[#This Row],[list from dll]])&gt;0</f>
@@ -9322,7 +9327,7 @@
     </row>
     <row r="170" spans="1:2">
       <c r="A170" t="s">
-        <v>771</v>
+        <v>760</v>
       </c>
       <c r="B170" s="3" t="b">
         <f>COUNTIF('Documentation list'!C:C,Table2[[#This Row],[list from dll]])&gt;0</f>
@@ -9340,7 +9345,7 @@
     </row>
     <row r="172" spans="1:2">
       <c r="A172" t="s">
-        <v>772</v>
+        <v>761</v>
       </c>
       <c r="B172" s="3" t="b">
         <f>COUNTIF('Documentation list'!C:C,Table2[[#This Row],[list from dll]])&gt;0</f>
@@ -9349,7 +9354,7 @@
     </row>
     <row r="173" spans="1:2">
       <c r="A173" t="s">
-        <v>773</v>
+        <v>762</v>
       </c>
       <c r="B173" s="3" t="b">
         <f>COUNTIF('Documentation list'!C:C,Table2[[#This Row],[list from dll]])&gt;0</f>

</xml_diff>

<commit_message>
Changed Zmanim Project to VB.Net Port
</commit_message>
<xml_diff>
--- a/Resources/ZmanimFunctionList.xlsx
+++ b/Resources/ZmanimFunctionList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub Project\MYZman\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23A90320-7E55-4BAF-A1FA-FBDA42A7929A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDF069AD-C1BA-44F9-95ED-8F44CDEC1BF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4125" yWindow="2430" windowWidth="26025" windowHeight="16680" xr2:uid="{67155520-7577-4C1A-98E8-EE8F939659DB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{67155520-7577-4C1A-98E8-EE8F939659DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Documentation list" sheetId="1" r:id="rId1"/>
@@ -3912,7 +3912,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:H167"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+    <sheetView zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -9416,8 +9416,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:D170"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="A75" sqref="A75"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>